<commit_message>
set data and upload
</commit_message>
<xml_diff>
--- a/app/static/Flu09/data_files_names.xlsx
+++ b/app/static/Flu09/data_files_names.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>patient_data_linear.xlsx</t>
+    <t>cytokine_data.xlsx</t>
   </si>
   <si>
-    <t>cytokine_data.xlsx</t>
+    <t>patient_data.xlsx</t>
+  </si>
+  <si>
+    <t>Flu09</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -404,6 +407,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>